<commit_message>
Testplan Done & Uploaded
</commit_message>
<xml_diff>
--- a/Documentation/Project_overall_individual_status_and_MoM/eiTRA_UVM_Project_Daily_Status_MoM.xlsx
+++ b/Documentation/Project_overall_individual_status_and_MoM/eiTRA_UVM_Project_Daily_Status_MoM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Project Status" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
   <si>
     <t xml:space="preserve">Sr No</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t xml:space="preserve">Validation &amp; Closure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">Date of Entry</t>
@@ -324,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -353,6 +350,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -379,7 +383,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -498,6 +502,10 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -611,22 +619,22 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -725,7 +733,9 @@
       <c r="I4" s="9" t="n">
         <v>45178</v>
       </c>
-      <c r="J4" s="12"/>
+      <c r="J4" s="12" t="n">
+        <v>45178</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -1295,20 +1305,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:D182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="65.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="55.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="65.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,61 +1333,237 @@
       <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="n">
+        <v>45147</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29" t="n">
-        <v>45147</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+    </row>
+    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+    </row>
+    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+    </row>
+    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+    </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1391,38 +1576,8 @@
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="54" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="83" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="84" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="85" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1433,22 +1588,15 @@
     <row r="90" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="101" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="177" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="178" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="179" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="180" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="182" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="183" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="184" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A11"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1480,90 +1628,90 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="30"/>
+      <c r="A1" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="34"/>
+        <v>53</v>
+      </c>
+      <c r="B6" s="35"/>
     </row>
     <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
     </row>
     <row r="8" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="37"/>
     </row>
     <row r="9" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="30" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="38" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="s">
+      <c r="B10" s="21"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="21"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="s">
+      <c r="B11" s="21"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="21"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="s">
+      <c r="B12" s="21"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="21"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="s">
+      <c r="B13" s="21"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="38" t="s">
         <v>60</v>
-      </c>
-      <c r="B13" s="21"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="s">
-        <v>61</v>
       </c>
       <c r="B14" s="21"/>
     </row>

</xml_diff>

<commit_message>
Update Daily Status and Added Top Module File
</commit_message>
<xml_diff>
--- a/Documentation/Project_overall_individual_status_and_MoM/eiTRA_UVM_Project_Daily_Status_MoM.xlsx
+++ b/Documentation/Project_overall_individual_status_and_MoM/eiTRA_UVM_Project_Daily_Status_MoM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Project Status" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
   <si>
     <t xml:space="preserve">Sr No</t>
   </si>
@@ -161,6 +161,13 @@
   </si>
   <si>
     <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed the Vplan and Testplan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Started Testplan with 21 testcases in line.
+2. Created initial Vplan with as details available currently.</t>
   </si>
   <si>
     <t xml:space="preserve">Can use different color coding for highlight</t>
@@ -383,7 +390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -500,12 +507,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -619,7 +638,7 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -1309,17 +1328,17 @@
   </sheetPr>
   <dimension ref="A1:D182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="65.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="20.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="41.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="65.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="29" width="55.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="29" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1336,8 +1355,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="n">
+    <row r="2" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="n">
         <v>45147</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1350,221 +1369,229 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+    <row r="3" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="31" t="n">
+        <v>45178</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
     </row>
     <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1630,90 +1657,90 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="31"/>
+      <c r="A1" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="35"/>
+        <v>55</v>
+      </c>
+      <c r="B6" s="38"/>
     </row>
     <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
     </row>
     <row r="8" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36"/>
-      <c r="B8" s="37"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
     </row>
     <row r="9" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="38" t="s">
-        <v>56</v>
+      <c r="A10" s="41" t="s">
+        <v>58</v>
       </c>
       <c r="B10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="38" t="s">
-        <v>57</v>
+      <c r="A11" s="41" t="s">
+        <v>59</v>
       </c>
       <c r="B11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="38" t="s">
-        <v>58</v>
+      <c r="A12" s="41" t="s">
+        <v>60</v>
       </c>
       <c r="B12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
-        <v>59</v>
+      <c r="A13" s="41" t="s">
+        <v>61</v>
       </c>
       <c r="B13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
-        <v>60</v>
+      <c r="A14" s="41" t="s">
+        <v>62</v>
       </c>
       <c r="B14" s="21"/>
     </row>

</xml_diff>